<commit_message>
quantifying proteins for b7, 2nd protein unfolding run
</commit_message>
<xml_diff>
--- a/Data/2018-07-20_prelim_homogenizatio_BCA.xlsx
+++ b/Data/2018-07-20_prelim_homogenizatio_BCA.xlsx
@@ -1,16 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19226"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hannahchu\Documents\GitHub\Proteome_stability_project\Data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDB532A0-F085-4D8F-872C-1F346E56C6D2}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14820" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="14820" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2018-07-20" sheetId="1" r:id="rId1"/>
     <sheet name="2018-07-23" sheetId="2" r:id="rId2"/>
+    <sheet name="2018-07-25" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="179017" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -20,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="22">
   <si>
     <t>Sample</t>
   </si>
@@ -84,11 +91,14 @@
   <si>
     <t>S10</t>
   </si>
+  <si>
+    <t>samp</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -158,11 +168,19 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -176,7 +194,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -209,7 +226,6 @@
             <c:dispRSqr val="0"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
             </c:trendlineLbl>
           </c:trendline>
@@ -226,13 +242,13 @@
                   <c:v>0.749</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.4545</c:v>
+                  <c:v>0.45449999999999996</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.1355</c:v>
+                  <c:v>0.13550000000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -244,10 +260,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>2.0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0.5</c:v>
@@ -256,12 +272,17 @@
                   <c:v>0.25</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-FBFD-480F-BBCF-2B1EB587DBB7}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -303,7 +324,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -337,7 +357,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -365,14 +384,14 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1" l="0.75" r="0.75" t="1" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -404,7 +423,6 @@
             <c:dispRSqr val="0"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
             </c:trendlineLbl>
           </c:trendline>
@@ -424,10 +442,10 @@
                   <c:v>0.746</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.471</c:v>
+                  <c:v>0.47099999999999992</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -439,10 +457,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>2.0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0.5</c:v>
@@ -451,12 +469,17 @@
                   <c:v>0.25</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-38A7-420D-8720-8EA2D0FDDD03}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -496,7 +519,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -535,7 +557,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -563,14 +584,14 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1" l="0.75" r="0.75" t="1" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -604,7 +625,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0.119</c:v>
+                  <c:v>0.11900000000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.1105</c:v>
@@ -613,30 +634,35 @@
                   <c:v>0.1085</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.095</c:v>
+                  <c:v>9.4999999999999987E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.094</c:v>
+                  <c:v>9.3999999999999986E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.0875</c:v>
+                  <c:v>8.7500000000000008E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.09</c:v>
+                  <c:v>8.9999999999999983E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.0855</c:v>
+                  <c:v>8.5500000000000007E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.088</c:v>
+                  <c:v>8.8000000000000009E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.092</c:v>
+                  <c:v>9.1999999999999985E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-D40D-4460-AEEA-720DCD2F1254}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -686,10 +712,927 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1" l="0.75" r="0.75" t="1" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'2018-07-25'!$E$2:$E$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1.9739999999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.1164999999999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.60300000000000009</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.31</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'2018-07-25'!$A$2:$A$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-13D8-4021-9851-F1B9C384F2EA}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="424342232"/>
+        <c:axId val="424336000"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="424342232"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="424336000"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="424336000"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="424342232"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -709,7 +1652,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -744,7 +1693,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -774,7 +1729,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -784,6 +1745,47 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>71437</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>138112</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E9116A61-0BEC-45A6-8255-28FEC1A12EE4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1113,19 +2115,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection sqref="A1:G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="7" max="7" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1148,7 +2150,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2</v>
       </c>
@@ -1167,7 +2169,7 @@
         <v>2.1555</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1186,7 +2188,7 @@
         <v>0.749</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>0.5</v>
       </c>
@@ -1197,7 +2199,7 @@
         <v>0.59499999999999997</v>
       </c>
       <c r="D4">
-        <f t="shared" ref="D3:D10" si="1">AVERAGE(B4:C4)</f>
+        <f t="shared" ref="D4:D10" si="1">AVERAGE(B4:C4)</f>
         <v>0.52649999999999997</v>
       </c>
       <c r="E4">
@@ -1205,7 +2207,7 @@
         <v>0.45449999999999996</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>0.25</v>
       </c>
@@ -1224,7 +2226,7 @@
         <v>0.13550000000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>0</v>
       </c>
@@ -1242,7 +2244,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -1269,7 +2271,7 @@
         <v>9.5287600000000028E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -1292,7 +2294,7 @@
         <v>0.51801439999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -1319,7 +2321,7 @@
         <v>0.15670519999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -1355,16 +2357,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1384,7 +2386,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2</v>
       </c>
@@ -1403,7 +2405,7 @@
         <v>2.641</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1422,7 +2424,7 @@
         <v>1.399</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>0.5</v>
       </c>
@@ -1441,7 +2443,7 @@
         <v>0.746</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>0.25</v>
       </c>
@@ -1460,7 +2462,7 @@
         <v>0.47099999999999992</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>0</v>
       </c>
@@ -1479,7 +2481,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -1502,7 +2504,7 @@
         <v>3.0256100000000008E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -1525,7 +2527,7 @@
         <v>2.3694950000000006E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -1548,7 +2550,7 @@
         <v>2.2151149999999994E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -1571,7 +2573,7 @@
         <v>1.1730499999999991E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -1594,7 +2596,7 @@
         <v>1.0958599999999985E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -1617,7 +2619,7 @@
         <v>5.941250000000009E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>17</v>
       </c>
@@ -1640,7 +2642,7 @@
         <v>7.8709999999999891E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>18</v>
       </c>
@@ -1663,7 +2665,7 @@
         <v>4.3974500000000111E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>19</v>
       </c>
@@ -1686,7 +2688,7 @@
         <v>6.327200000000005E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>20</v>
       </c>
@@ -1718,4 +2720,185 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33093A63-4EE6-49B7-A537-6BD672D1243E}">
+  <dimension ref="A1:F7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="7.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="5.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>2.3559999999999999</v>
+      </c>
+      <c r="C2">
+        <v>1.736</v>
+      </c>
+      <c r="D2">
+        <f>AVERAGE(B2:C2)</f>
+        <v>2.0459999999999998</v>
+      </c>
+      <c r="E2">
+        <f>D2-$D$6</f>
+        <v>1.9739999999999998</v>
+      </c>
+      <c r="F2">
+        <f>(1.0182*E2) - 0.0652</f>
+        <v>1.9447267999999998</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>1.1659999999999999</v>
+      </c>
+      <c r="C3">
+        <v>1.2110000000000001</v>
+      </c>
+      <c r="D3">
+        <f>AVERAGE(B3:C3)</f>
+        <v>1.1884999999999999</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ref="E3:E7" si="0">D3-$D$6</f>
+        <v>1.1164999999999998</v>
+      </c>
+      <c r="F3">
+        <f>(1.0182*E3) - 0.0652</f>
+        <v>1.0716203</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>0.5</v>
+      </c>
+      <c r="B4">
+        <v>0.68100000000000005</v>
+      </c>
+      <c r="C4">
+        <v>0.66900000000000004</v>
+      </c>
+      <c r="D4">
+        <f t="shared" ref="D4:D5" si="1">AVERAGE(B4:C4)</f>
+        <v>0.67500000000000004</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="0"/>
+        <v>0.60300000000000009</v>
+      </c>
+      <c r="F4">
+        <f>(1.0182*E4) - 0.0652</f>
+        <v>0.5487746</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>0.25</v>
+      </c>
+      <c r="B5">
+        <v>0.39</v>
+      </c>
+      <c r="C5">
+        <v>0.374</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="1"/>
+        <v>0.38200000000000001</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>0.31</v>
+      </c>
+      <c r="F5">
+        <f>(1.0182*E5) - 0.0652</f>
+        <v>0.250442</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>0</v>
+      </c>
+      <c r="B6">
+        <v>6.8000000000000005E-2</v>
+      </c>
+      <c r="C6">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="D6">
+        <v>7.1999999999999995E-2</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <f>(1.0182*E6) - 0.0652</f>
+        <v>-6.5199999999999994E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7">
+        <v>0.76700000000000002</v>
+      </c>
+      <c r="C7">
+        <v>0.78200000000000003</v>
+      </c>
+      <c r="D7">
+        <f>AVERAGE(B7:C7)</f>
+        <v>0.77449999999999997</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>0.70250000000000001</v>
+      </c>
+      <c r="F7">
+        <f>(1.0182*E7) - 0.0652</f>
+        <v>0.65008549999999998</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>